<commit_message>
ENHANCE: Allow specifying accessLevel as any string, fix typos
</commit_message>
<xml_diff>
--- a/Sample/campus.xlsx
+++ b/Sample/campus.xlsx
@@ -115,25 +115,25 @@
     <t xml:space="preserve">servedBy</t>
   </si>
   <si>
-    <t xml:space="preserve">{"accessLevel": 0.75, "availability": 99.0, "failMode": "failclose"}</t>
+    <t xml:space="preserve">{"accessLevel": "visitor", "availability": 99.0, "failMode": "failclosed"}</t>
   </si>
   <si>
     <t xml:space="preserve">AccessReaderE2O</t>
   </si>
   <si>
-    <t xml:space="preserve">{"accessLevel": 0.5, "availability": 90.0, "failMode": "failclose"}</t>
+    <t xml:space="preserve">{"accessLevel": "staff", "availability": 90.0, "failMode": "failclosed"}</t>
   </si>
   <si>
     <t xml:space="preserve">AccessReaderS2O</t>
   </si>
   <si>
-    <t xml:space="preserve">{"accessLevel": 0.5, "availability": 98.0,  "failMode": "failopen"}</t>
+    <t xml:space="preserve">{"accessLevel": "staff", "availability": 98.0,  "failMode": "failopen"}</t>
   </si>
   <si>
     <t xml:space="preserve">AccessReaderS2R</t>
   </si>
   <si>
-    <t xml:space="preserve">{"accessLevel": 0.25, "availability": 80.0, "failMode": "failclose"}</t>
+    <t xml:space="preserve">{"accessLevel": "security", "availability": 80.0, "failMode": "failclosed"}</t>
   </si>
   <si>
     <t xml:space="preserve">dtmi:au:edu:deakin:a2i2:SurveillanceCamera;1</t>
@@ -252,7 +252,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
ENHANCE: Attach Microphones to sample Campus
</commit_message>
<xml_diff>
--- a/Sample/campus.xlsx
+++ b/Sample/campus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
   <si>
     <t xml:space="preserve">ModelID</t>
   </si>
@@ -100,6 +100,12 @@
     <t xml:space="preserve">S2R</t>
   </si>
   <si>
+    <t xml:space="preserve">dtmi:digitaltwins:rec_3_3:asset:Window;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2C</t>
+  </si>
+  <si>
     <t xml:space="preserve">fromSpace</t>
   </si>
   <si>
@@ -149,6 +155,39 @@
   </si>
   <si>
     <t xml:space="preserve">{"privacyCost": 1.0, "availability": 75.0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dtmi:au:edu:deakin:a2i2:SurveillanceMicrophone;1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mic1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"privacyCost": 1.0, "availability": 50.0, "p_speech": 0, "p_glass": 0, "p_silence": 0}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mic2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mic3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mica74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micp3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micnp6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micn10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mics21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">micq7</t>
   </si>
 </sst>
 </file>
@@ -158,12 +197,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,6 +217,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,13 +267,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -249,10 +297,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -404,25 +452,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,21 +475,21 @@
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,46 +497,45 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,147 +544,334 @@
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="0" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>42</v>
+      <c r="D34" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ENHANCE: Represent attack from Roof
</commit_message>
<xml_diff>
--- a/Sample/campus.xlsx
+++ b/Sample/campus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="57">
   <si>
     <t xml:space="preserve">ModelID</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">dtmi:digitaltwins:rec_3_3:asset:Window;1</t>
   </si>
   <si>
-    <t xml:space="preserve">O2C</t>
+    <t xml:space="preserve">R2O</t>
   </si>
   <si>
     <t xml:space="preserve">fromSpace</t>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t xml:space="preserve">micq7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SurveillanceS2O</t>
   </si>
 </sst>
 </file>
@@ -197,11 +200,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -217,12 +221,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,11 +270,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,10 +295,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -599,7 +597,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>27</v>
@@ -610,7 +608,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>27</v>
@@ -872,6 +870,23 @@
       </c>
       <c r="E43" s="0" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>